<commit_message>
Validated conven and initiated kernza2
Tweaked crops in conventional simulation and calculated RMSEs, then
introduced a new schedule file "kernza2" that includs IWG, and it works.
Grain yields are a bit low, need to look at ANPP.
</commit_message>
<xml_diff>
--- a/simulations/Convertingcgrain2yieldV2.xlsx
+++ b/simulations/Convertingcgrain2yieldV2.xlsx
@@ -18,7 +18,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">conven!$A$1:$K$1143</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -900,7 +900,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A1139" sqref="A10:K1139"/>
+      <selection pane="bottomLeft" activeCell="C166" sqref="C166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37726,7 +37726,7 @@
   <dimension ref="A1:U76"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+      <selection activeCell="O3" sqref="O3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -37888,11 +37888,11 @@
         <v>17</v>
       </c>
       <c r="M3">
-        <f>F3/0.48</f>
+        <f t="shared" ref="M2:M11" si="0">F3/0.48</f>
         <v>330.86500000000001</v>
       </c>
       <c r="N3">
-        <f t="shared" ref="N3:N69" si="0">M3*10</f>
+        <f t="shared" ref="N3:N69" si="1">M3*10</f>
         <v>3308.65</v>
       </c>
       <c r="O3">
@@ -37900,7 +37900,7 @@
         <v>3379.2565910000003</v>
       </c>
       <c r="P3">
-        <f t="shared" ref="P3:P11" si="1">O3/48</f>
+        <f t="shared" ref="P3:P11" si="2">O3/48</f>
         <v>70.401178979166673</v>
       </c>
       <c r="R3" t="s">
@@ -37951,19 +37951,19 @@
         <v>17</v>
       </c>
       <c r="M4">
-        <f>F4/0.48</f>
+        <f t="shared" si="0"/>
         <v>360.06416666666672</v>
       </c>
       <c r="N4">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3600.6416666666673</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O11" si="2">(M4*1.145)*8.92</f>
+        <f t="shared" ref="O4:O11" si="3">(M4*1.145)*8.92</f>
         <v>3677.479359833334</v>
       </c>
       <c r="P4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>76.614153329861125</v>
       </c>
       <c r="R4" t="s">
@@ -37973,7 +37973,7 @@
         <v>0.46</v>
       </c>
       <c r="T4">
-        <v>1.4E-2</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="U4">
         <v>32</v>
@@ -38014,19 +38014,19 @@
         <v>17</v>
       </c>
       <c r="M5">
-        <f>F5/0.48</f>
+        <f t="shared" si="0"/>
         <v>343.28562499999998</v>
       </c>
       <c r="N5">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3432.8562499999998</v>
       </c>
       <c r="O5">
+        <f t="shared" si="3"/>
+        <v>3506.1134023750001</v>
+      </c>
+      <c r="P5">
         <f t="shared" si="2"/>
-        <v>3506.1134023750001</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="1"/>
         <v>73.04402921614583</v>
       </c>
       <c r="R5" t="s">
@@ -38077,19 +38077,19 @@
         <v>17</v>
       </c>
       <c r="M6">
-        <f>F6/0.48</f>
+        <f t="shared" si="0"/>
         <v>379.08229166666666</v>
       </c>
       <c r="N6">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3790.8229166666665</v>
       </c>
       <c r="O6">
+        <f t="shared" si="3"/>
+        <v>3871.7190777083333</v>
+      </c>
+      <c r="P6">
         <f t="shared" si="2"/>
-        <v>3871.7190777083333</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="1"/>
         <v>80.660814118923611</v>
       </c>
       <c r="R6" t="s">
@@ -38140,19 +38140,19 @@
         <v>17</v>
       </c>
       <c r="M7">
-        <f>F7/0.48</f>
+        <f t="shared" si="0"/>
         <v>470.94666666666666</v>
       </c>
       <c r="N7">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4709.4666666666662</v>
       </c>
       <c r="O7">
+        <f t="shared" si="3"/>
+        <v>4809.9666853333329</v>
+      </c>
+      <c r="P7">
         <f t="shared" si="2"/>
-        <v>4809.9666853333329</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="1"/>
         <v>100.20763927777777</v>
       </c>
     </row>
@@ -38191,19 +38191,19 @@
         <v>17</v>
       </c>
       <c r="M8">
-        <f>F8/0.48</f>
+        <f t="shared" si="0"/>
         <v>503.43645833333335</v>
       </c>
       <c r="N8">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5034.3645833333339</v>
       </c>
       <c r="O8">
+        <f t="shared" si="3"/>
+        <v>5141.7979235416669</v>
+      </c>
+      <c r="P8">
         <f t="shared" si="2"/>
-        <v>5141.7979235416669</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="1"/>
         <v>107.12079007378473</v>
       </c>
     </row>
@@ -38242,19 +38242,19 @@
         <v>17</v>
       </c>
       <c r="M9">
-        <f>F9/0.48</f>
+        <f t="shared" si="0"/>
         <v>436.01958333333334</v>
       </c>
       <c r="N9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4360.1958333333332</v>
       </c>
       <c r="O9">
+        <f t="shared" si="3"/>
+        <v>4453.2424124166664</v>
+      </c>
+      <c r="P9">
         <f t="shared" si="2"/>
-        <v>4453.2424124166664</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="1"/>
         <v>92.775883592013884</v>
       </c>
     </row>
@@ -38293,19 +38293,19 @@
         <v>17</v>
       </c>
       <c r="M10">
-        <f>F10/0.48</f>
+        <f t="shared" si="0"/>
         <v>554.21979166666677</v>
       </c>
       <c r="N10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5542.1979166666679</v>
       </c>
       <c r="O10">
+        <f t="shared" si="3"/>
+        <v>5660.4684202083345</v>
+      </c>
+      <c r="P10">
         <f t="shared" si="2"/>
-        <v>5660.4684202083345</v>
-      </c>
-      <c r="P10">
-        <f t="shared" si="1"/>
         <v>117.92642542100697</v>
       </c>
     </row>
@@ -38344,19 +38344,19 @@
         <v>17</v>
       </c>
       <c r="M11">
-        <f>F11/0.48</f>
+        <f t="shared" si="0"/>
         <v>574.99458333333337</v>
       </c>
       <c r="N11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5749.9458333333332</v>
       </c>
       <c r="O11">
+        <f t="shared" si="3"/>
+        <v>5872.6496774166671</v>
+      </c>
+      <c r="P11">
         <f t="shared" si="2"/>
-        <v>5872.6496774166671</v>
-      </c>
-      <c r="P11">
-        <f t="shared" si="1"/>
         <v>122.3468682795139</v>
       </c>
     </row>
@@ -38399,7 +38399,7 @@
         <v>622.66155555555554</v>
       </c>
       <c r="N12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6226.6155555555551</v>
       </c>
       <c r="O12">
@@ -38446,19 +38446,19 @@
         <v>10</v>
       </c>
       <c r="M13">
-        <f t="shared" ref="M13:M17" si="3">F13/0.45</f>
+        <f t="shared" ref="M13:M17" si="4">F13/0.45</f>
         <v>612.03511111111106</v>
       </c>
       <c r="N13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>6120.3511111111111</v>
       </c>
       <c r="O13">
-        <f t="shared" ref="O13:O18" si="4">(M13*1.155)*8.92</f>
+        <f t="shared" ref="O13:O18" si="5">(M13*1.155)*8.92</f>
         <v>6305.5529357333326</v>
       </c>
       <c r="P13">
-        <f t="shared" ref="P13:P18" si="5">O13/56</f>
+        <f t="shared" ref="P13:P18" si="6">O13/56</f>
         <v>112.59915956666666</v>
       </c>
     </row>
@@ -38497,19 +38497,19 @@
         <v>10</v>
       </c>
       <c r="M14">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>486.64955555555554</v>
       </c>
       <c r="N14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4866.4955555555553</v>
       </c>
       <c r="O14">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5013.7557110666667</v>
       </c>
       <c r="P14">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>89.531351983333337</v>
       </c>
     </row>
@@ -38548,19 +38548,19 @@
         <v>10</v>
       </c>
       <c r="M15">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>807.32266666666669</v>
       </c>
       <c r="N15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>8073.2266666666674</v>
       </c>
       <c r="O15">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>8317.5225055999999</v>
       </c>
       <c r="P15">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>148.52718759999999</v>
       </c>
     </row>
@@ -38599,19 +38599,19 @@
         <v>10</v>
       </c>
       <c r="M16">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>772.40266666666673</v>
       </c>
       <c r="N16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>7724.0266666666676</v>
       </c>
       <c r="O16">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>7957.7557136000014</v>
       </c>
       <c r="P16">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>142.10278060000002</v>
       </c>
     </row>
@@ -38650,19 +38650,19 @@
         <v>10</v>
       </c>
       <c r="M17">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>547.88377777777771</v>
       </c>
       <c r="N17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5478.8377777777769</v>
       </c>
       <c r="O17">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5644.6274089333328</v>
       </c>
       <c r="P17">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>100.79691801666665</v>
       </c>
     </row>
@@ -38701,19 +38701,19 @@
         <v>10</v>
       </c>
       <c r="M18">
-        <f t="shared" ref="M18" si="6">F18/0.45</f>
+        <f t="shared" ref="M18" si="7">F18/0.45</f>
         <v>532.18355555555547</v>
       </c>
       <c r="N18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5321.8355555555545</v>
       </c>
       <c r="O18">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>5482.8742994666654</v>
       </c>
       <c r="P18">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>97.908469633333311</v>
       </c>
     </row>
@@ -38752,11 +38752,11 @@
         <v>18</v>
       </c>
       <c r="M19">
-        <f>F18/0.46</f>
+        <f t="shared" ref="M19:M28" si="8">F18/0.46</f>
         <v>520.61434782608694</v>
       </c>
       <c r="N19">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>5206.1434782608694</v>
       </c>
       <c r="O19">
@@ -38803,19 +38803,19 @@
         <v>18</v>
       </c>
       <c r="M20">
-        <f>F19/0.46</f>
+        <f t="shared" si="8"/>
         <v>45.912173913043475</v>
       </c>
       <c r="N20">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>459.12173913043478</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:O28" si="7">(M20*1.14)*8.92</f>
+        <f t="shared" ref="O20:O28" si="9">(M20*1.14)*8.92</f>
         <v>466.87171408695644</v>
       </c>
       <c r="P20">
-        <f t="shared" ref="P20:P28" si="8">O20/32</f>
+        <f t="shared" ref="P20:P28" si="10">O20/32</f>
         <v>14.589741065217389</v>
       </c>
     </row>
@@ -38854,19 +38854,19 @@
         <v>18</v>
       </c>
       <c r="M21">
-        <f>F20/0.46</f>
+        <f t="shared" si="8"/>
         <v>46.074782608695656</v>
       </c>
       <c r="N21">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>460.74782608695659</v>
       </c>
       <c r="O21">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>468.52524939130438</v>
       </c>
       <c r="P21">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>14.641414043478262</v>
       </c>
     </row>
@@ -38905,19 +38905,19 @@
         <v>18</v>
       </c>
       <c r="M22">
-        <f>F21/0.46</f>
+        <f t="shared" si="8"/>
         <v>56.059347826086949</v>
       </c>
       <c r="N22">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>560.59347826086946</v>
       </c>
       <c r="O22">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>570.05629617391287</v>
       </c>
       <c r="P22">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>17.814259255434777</v>
       </c>
     </row>
@@ -38956,19 +38956,19 @@
         <v>18</v>
       </c>
       <c r="M23">
-        <f>F22/0.46</f>
+        <f t="shared" si="8"/>
         <v>89.849347826086955</v>
       </c>
       <c r="N23">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>898.49347826086955</v>
       </c>
       <c r="O23">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>913.66004817391286</v>
       </c>
       <c r="P23">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>28.551876505434777</v>
       </c>
     </row>
@@ -39007,19 +39007,19 @@
         <v>18</v>
       </c>
       <c r="M24">
-        <f>F23/0.46</f>
+        <f t="shared" si="8"/>
         <v>82.298260869565212</v>
       </c>
       <c r="N24">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>822.98260869565206</v>
       </c>
       <c r="O24">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>836.8745551304346</v>
       </c>
       <c r="P24">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>26.152329847826081</v>
       </c>
     </row>
@@ -39058,19 +39058,19 @@
         <v>18</v>
       </c>
       <c r="M25">
-        <f>F24/0.46</f>
+        <f t="shared" si="8"/>
         <v>124.24</v>
       </c>
       <c r="N25">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1242.3999999999999</v>
       </c>
       <c r="O25">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>1263.3717119999997</v>
       </c>
       <c r="P25">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>39.480365999999989</v>
       </c>
     </row>
@@ -39109,19 +39109,19 @@
         <v>18</v>
       </c>
       <c r="M26">
-        <f>F25/0.46</f>
+        <f t="shared" si="8"/>
         <v>74.536521739130436</v>
       </c>
       <c r="N26">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>745.36521739130433</v>
       </c>
       <c r="O26">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>757.9469822608695</v>
       </c>
       <c r="P26">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>23.685843195652172</v>
       </c>
     </row>
@@ -39160,19 +39160,19 @@
         <v>18</v>
       </c>
       <c r="M27">
-        <f>F26/0.46</f>
+        <f t="shared" si="8"/>
         <v>70.130869565217381</v>
       </c>
       <c r="N27">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>701.30869565217381</v>
       </c>
       <c r="O27">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>713.14678643478237</v>
       </c>
       <c r="P27">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>22.285837076086949</v>
       </c>
     </row>
@@ -39211,19 +39211,19 @@
         <v>18</v>
       </c>
       <c r="M28">
-        <f>F27/0.46</f>
+        <f t="shared" si="8"/>
         <v>41.238913043478256</v>
       </c>
       <c r="N28">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>412.38913043478254</v>
       </c>
       <c r="O28">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>419.35025895652166</v>
       </c>
       <c r="P28">
-        <f t="shared" si="8"/>
+        <f t="shared" si="10"/>
         <v>13.104695592391302</v>
       </c>
     </row>
@@ -39262,11 +39262,11 @@
         <v>12</v>
       </c>
       <c r="M29">
-        <f>F28/0.54</f>
+        <f t="shared" ref="M29:M43" si="11">F28/0.54</f>
         <v>95.514999999999986</v>
       </c>
       <c r="N29">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>955.14999999999986</v>
       </c>
       <c r="O29">
@@ -39313,11 +39313,11 @@
         <v>12</v>
       </c>
       <c r="M30">
-        <f>F29/0.54</f>
+        <f t="shared" si="11"/>
         <v>129.20074074074074</v>
       </c>
       <c r="N30">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1292.0074074074073</v>
       </c>
       <c r="O30">
@@ -39325,7 +39325,7 @@
         <v>1302.2917863703701</v>
       </c>
       <c r="P30">
-        <f t="shared" ref="P30:P76" si="9">O30/60</f>
+        <f t="shared" ref="P30:P76" si="12">O30/60</f>
         <v>21.704863106172834</v>
       </c>
     </row>
@@ -39364,19 +39364,19 @@
         <v>12</v>
       </c>
       <c r="M31">
-        <f>F30/0.54</f>
+        <f t="shared" si="11"/>
         <v>151.54</v>
       </c>
       <c r="N31">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1515.3999999999999</v>
       </c>
       <c r="O31">
-        <f t="shared" ref="O31:O43" si="10">(M31*1.13)*8.92</f>
+        <f t="shared" ref="O31:O43" si="13">(M31*1.13)*8.92</f>
         <v>1527.4625839999999</v>
       </c>
       <c r="P31">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>25.457709733333331</v>
       </c>
     </row>
@@ -39415,19 +39415,19 @@
         <v>12</v>
       </c>
       <c r="M32">
-        <f>F31/0.54</f>
+        <f t="shared" si="11"/>
         <v>171.05388888888888</v>
       </c>
       <c r="N32">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1710.5388888888888</v>
       </c>
       <c r="O32">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1724.154778444444</v>
       </c>
       <c r="P32">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>28.735912974074065</v>
       </c>
     </row>
@@ -39466,19 +39466,19 @@
         <v>12</v>
       </c>
       <c r="M33">
-        <f>F32/0.54</f>
+        <f t="shared" si="11"/>
         <v>228.42092592592593</v>
       </c>
       <c r="N33">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2284.2092592592594</v>
       </c>
       <c r="O33">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2302.391564962963</v>
       </c>
       <c r="P33">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>38.373192749382717</v>
       </c>
     </row>
@@ -39517,19 +39517,19 @@
         <v>12</v>
       </c>
       <c r="M34">
-        <f>F33/0.54</f>
+        <f t="shared" si="11"/>
         <v>225.71222222222221</v>
       </c>
       <c r="N34">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2257.1222222222223</v>
       </c>
       <c r="O34">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2275.0889151111105</v>
       </c>
       <c r="P34">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>37.918148585185172</v>
       </c>
     </row>
@@ -39568,19 +39568,19 @@
         <v>12</v>
       </c>
       <c r="M35">
-        <f>F34/0.54</f>
+        <f t="shared" si="11"/>
         <v>236.97296296296295</v>
       </c>
       <c r="N35">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2369.7296296296295</v>
       </c>
       <c r="O35">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2388.5926774814811</v>
       </c>
       <c r="P35">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>39.809877958024686</v>
       </c>
     </row>
@@ -39619,19 +39619,19 @@
         <v>12</v>
       </c>
       <c r="M36">
-        <f>F35/0.54</f>
+        <f t="shared" si="11"/>
         <v>135.52185185185184</v>
       </c>
       <c r="N36">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1355.2185185185183</v>
       </c>
       <c r="O36">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1366.0060579259255</v>
       </c>
       <c r="P36">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>22.766767632098759</v>
       </c>
     </row>
@@ -39670,19 +39670,19 @@
         <v>12</v>
       </c>
       <c r="M37">
-        <f>F36/0.54</f>
+        <f t="shared" si="11"/>
         <v>271.98185185185184</v>
       </c>
       <c r="N37">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2719.8185185185184</v>
       </c>
       <c r="O37">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2741.4682739259256</v>
       </c>
       <c r="P37">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>45.691137898765426</v>
       </c>
     </row>
@@ -39721,19 +39721,19 @@
         <v>12</v>
       </c>
       <c r="M38">
-        <f>F37/0.54</f>
+        <f t="shared" si="11"/>
         <v>221.56222222222223</v>
       </c>
       <c r="N38">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2215.6222222222223</v>
       </c>
       <c r="O38">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2233.258575111111</v>
       </c>
       <c r="P38">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>37.220976251851852</v>
       </c>
     </row>
@@ -39772,19 +39772,19 @@
         <v>12</v>
       </c>
       <c r="M39">
-        <f>F38/0.54</f>
+        <f t="shared" si="11"/>
         <v>152.93314814814815</v>
       </c>
       <c r="N39">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1529.3314814814814</v>
       </c>
       <c r="O39">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1541.504960074074</v>
       </c>
       <c r="P39">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>25.691749334567898</v>
       </c>
     </row>
@@ -39823,19 +39823,19 @@
         <v>12</v>
       </c>
       <c r="M40">
-        <f>F39/0.54</f>
+        <f t="shared" si="11"/>
         <v>151.0338888888889</v>
       </c>
       <c r="N40">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1510.338888888889</v>
       </c>
       <c r="O40">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1522.3611864444442</v>
       </c>
       <c r="P40">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>25.372686440740736</v>
       </c>
     </row>
@@ -39874,19 +39874,19 @@
         <v>12</v>
       </c>
       <c r="M41">
-        <f>F40/0.54</f>
+        <f t="shared" si="11"/>
         <v>197.91740740740738</v>
       </c>
       <c r="N41">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1979.1740740740738</v>
       </c>
       <c r="O41">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>1994.9282997037033</v>
       </c>
       <c r="P41">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>33.248804995061718</v>
       </c>
     </row>
@@ -39925,19 +39925,19 @@
         <v>12</v>
       </c>
       <c r="M42">
-        <f>F41/0.54</f>
+        <f t="shared" si="11"/>
         <v>201.35351851851851</v>
       </c>
       <c r="N42">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2013.5351851851851</v>
       </c>
       <c r="O42">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2029.5629252592591</v>
       </c>
       <c r="P42">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>33.826048754320986</v>
       </c>
     </row>
@@ -39976,19 +39976,19 @@
         <v>12</v>
       </c>
       <c r="M43">
-        <f>F42/0.54</f>
+        <f t="shared" si="11"/>
         <v>225.43851851851852</v>
       </c>
       <c r="N43">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2254.385185185185</v>
       </c>
       <c r="O43">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>2272.330091259259</v>
       </c>
       <c r="P43">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>37.872168187654317</v>
       </c>
     </row>
@@ -40027,19 +40027,19 @@
         <v>12</v>
       </c>
       <c r="M44">
-        <f t="shared" ref="M44:M45" si="11">F43/0.54</f>
+        <f t="shared" ref="M44:M45" si="14">F43/0.54</f>
         <v>200.22259259259258</v>
       </c>
       <c r="N44">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2002.2259259259258</v>
       </c>
       <c r="O44">
-        <f t="shared" ref="O44:O45" si="12">(M44*1.13)*8.92</f>
+        <f t="shared" ref="O44:O45" si="15">(M44*1.13)*8.92</f>
         <v>2018.1636442962961</v>
       </c>
       <c r="P44">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>33.636060738271603</v>
       </c>
     </row>
@@ -40078,19 +40078,19 @@
         <v>12</v>
       </c>
       <c r="M45">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>129.97537037037037</v>
       </c>
       <c r="N45">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1299.7537037037036</v>
       </c>
       <c r="O45">
+        <f t="shared" si="15"/>
+        <v>1310.0997431851849</v>
+      </c>
+      <c r="P45">
         <f t="shared" si="12"/>
-        <v>1310.0997431851849</v>
-      </c>
-      <c r="P45">
-        <f t="shared" si="9"/>
         <v>21.834995719753081</v>
       </c>
     </row>
@@ -40129,11 +40129,11 @@
         <v>11</v>
       </c>
       <c r="M46">
-        <f>F43/0.46</f>
+        <f t="shared" ref="M46:M76" si="16">F43/0.46</f>
         <v>235.04391304347826</v>
       </c>
       <c r="N46">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2350.4391304347828</v>
       </c>
       <c r="O46">
@@ -40141,7 +40141,7 @@
         <v>2379.6315844347828</v>
       </c>
       <c r="P46">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>39.66052640724638</v>
       </c>
     </row>
@@ -40180,19 +40180,19 @@
         <v>11</v>
       </c>
       <c r="M47">
-        <f>F44/0.46</f>
+        <f t="shared" si="16"/>
         <v>152.57978260869564</v>
       </c>
       <c r="N47">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1525.7978260869563</v>
       </c>
       <c r="O47">
-        <f t="shared" ref="O47:O76" si="13">(M47*1.135)*8.92</f>
+        <f t="shared" ref="O47:O76" si="17">(M47*1.135)*8.92</f>
         <v>1544.7482350869564</v>
       </c>
       <c r="P47">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>25.745803918115939</v>
       </c>
     </row>
@@ -40231,19 +40231,19 @@
         <v>11</v>
       </c>
       <c r="M48">
-        <f>F45/0.46</f>
+        <f t="shared" si="16"/>
         <v>202.79</v>
       </c>
       <c r="N48">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2027.8999999999999</v>
       </c>
       <c r="O48">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2053.0865180000001</v>
       </c>
       <c r="P48">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>34.218108633333337</v>
       </c>
     </row>
@@ -40282,19 +40282,19 @@
         <v>11</v>
       </c>
       <c r="M49">
-        <f>F46/0.46</f>
+        <f t="shared" si="16"/>
         <v>37.143260869565211</v>
       </c>
       <c r="N49">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>371.43260869565211</v>
       </c>
       <c r="O49">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>376.04580169565207</v>
       </c>
       <c r="P49">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>6.2674300282608675</v>
       </c>
     </row>
@@ -40333,19 +40333,19 @@
         <v>11</v>
       </c>
       <c r="M50">
-        <f>F47/0.46</f>
+        <f t="shared" si="16"/>
         <v>110.07782608695652</v>
       </c>
       <c r="N50">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1100.7782608695652</v>
       </c>
       <c r="O50">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1114.4499268695652</v>
       </c>
       <c r="P50">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>18.574165447826086</v>
       </c>
     </row>
@@ -40384,19 +40384,19 @@
         <v>11</v>
       </c>
       <c r="M51">
-        <f>F48/0.46</f>
+        <f t="shared" si="16"/>
         <v>123.68652173913043</v>
       </c>
       <c r="N51">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1236.8652173913042</v>
       </c>
       <c r="O51">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1252.2270833913042</v>
       </c>
       <c r="P51">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>20.87045138985507</v>
       </c>
     </row>
@@ -40435,19 +40435,19 @@
         <v>11</v>
       </c>
       <c r="M52">
-        <f>F49/0.46</f>
+        <f t="shared" si="16"/>
         <v>147.46152173913043</v>
       </c>
       <c r="N52">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1474.6152173913042</v>
       </c>
       <c r="O52">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1492.9299383913044</v>
       </c>
       <c r="P52">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>24.882165639855074</v>
       </c>
     </row>
@@ -40486,19 +40486,19 @@
         <v>11</v>
       </c>
       <c r="M53">
-        <f>F50/0.46</f>
+        <f t="shared" si="16"/>
         <v>178.80565217391305</v>
       </c>
       <c r="N53">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1788.0565217391304</v>
       </c>
       <c r="O53">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1810.2641837391304</v>
       </c>
       <c r="P53">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>30.171069728985508</v>
       </c>
     </row>
@@ -40537,19 +40537,19 @@
         <v>11</v>
       </c>
       <c r="M54">
-        <f>F51/0.46</f>
+        <f t="shared" si="16"/>
         <v>215.22891304347826</v>
       </c>
       <c r="N54">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2152.2891304347827</v>
       </c>
       <c r="O54">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2179.0205614347824</v>
       </c>
       <c r="P54">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>36.31700935724637</v>
       </c>
     </row>
@@ -40588,19 +40588,19 @@
         <v>11</v>
       </c>
       <c r="M55">
-        <f>F52/0.46</f>
+        <f t="shared" si="16"/>
         <v>164.58391304347828</v>
       </c>
       <c r="N55">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1645.8391304347829</v>
       </c>
       <c r="O55">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1666.2804524347828</v>
       </c>
       <c r="P55">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>27.771340873913047</v>
       </c>
     </row>
@@ -40639,19 +40639,19 @@
         <v>11</v>
       </c>
       <c r="M56">
-        <f>F53/0.46</f>
+        <f t="shared" si="16"/>
         <v>203.48347826086956</v>
       </c>
       <c r="N56">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2034.8347826086956</v>
       </c>
       <c r="O56">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2060.1074306086957</v>
       </c>
       <c r="P56">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>34.335123843478264</v>
       </c>
     </row>
@@ -40690,19 +40690,19 @@
         <v>11</v>
       </c>
       <c r="M57">
-        <f>F54/0.46</f>
+        <f t="shared" si="16"/>
         <v>173.30130434782606</v>
       </c>
       <c r="N57">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1733.0130434782607</v>
       </c>
       <c r="O57">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1754.5370654782605</v>
       </c>
       <c r="P57">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>29.242284424637674</v>
       </c>
     </row>
@@ -40741,19 +40741,19 @@
         <v>11</v>
       </c>
       <c r="M58">
-        <f>F55/0.46</f>
+        <f t="shared" si="16"/>
         <v>162.41130434782607</v>
       </c>
       <c r="N58">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1624.1130434782608</v>
       </c>
       <c r="O58">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1644.2845274782608</v>
       </c>
       <c r="P58">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>27.404742124637679</v>
       </c>
     </row>
@@ -40792,19 +40792,19 @@
         <v>11</v>
       </c>
       <c r="M59">
-        <f>F56/0.46</f>
+        <f t="shared" si="16"/>
         <v>166.27108695652174</v>
       </c>
       <c r="N59">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1662.7108695652173</v>
       </c>
       <c r="O59">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1683.3617385652174</v>
       </c>
       <c r="P59">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>28.056028976086957</v>
       </c>
     </row>
@@ -40843,19 +40843,19 @@
         <v>11</v>
       </c>
       <c r="M60">
-        <f>F57/0.46</f>
+        <f t="shared" si="16"/>
         <v>131.98130434782607</v>
       </c>
       <c r="N60">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1319.8130434782606</v>
       </c>
       <c r="O60">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>1336.2051214782607</v>
       </c>
       <c r="P60">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>22.270085357971013</v>
       </c>
     </row>
@@ -40894,19 +40894,19 @@
         <v>11</v>
       </c>
       <c r="M61">
-        <f>F58/0.46</f>
+        <f t="shared" si="16"/>
         <v>221.79456521739129</v>
       </c>
       <c r="N61">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2217.945652173913</v>
       </c>
       <c r="O61">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2245.4925371739132</v>
       </c>
       <c r="P61">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>37.424875619565221</v>
       </c>
     </row>
@@ -40945,19 +40945,19 @@
         <v>11</v>
       </c>
       <c r="M62">
-        <f>F59/0.46</f>
+        <f t="shared" si="16"/>
         <v>241.47717391304346</v>
       </c>
       <c r="N62">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2414.7717391304345</v>
       </c>
       <c r="O62">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2444.7632041304341</v>
       </c>
       <c r="P62">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>40.746053402173899</v>
       </c>
     </row>
@@ -40996,19 +40996,19 @@
         <v>11</v>
       </c>
       <c r="M63">
-        <f>F60/0.46</f>
+        <f t="shared" si="16"/>
         <v>288.16195652173911</v>
       </c>
       <c r="N63">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2881.619565217391</v>
       </c>
       <c r="O63">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2917.4092802173909</v>
       </c>
       <c r="P63">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>48.62348800362318</v>
       </c>
     </row>
@@ -41047,19 +41047,19 @@
         <v>11</v>
       </c>
       <c r="M64">
-        <f>F61/0.46</f>
+        <f t="shared" si="16"/>
         <v>280.16195652173917</v>
       </c>
       <c r="N64">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2801.6195652173919</v>
       </c>
       <c r="O64">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2836.4156802173916</v>
       </c>
       <c r="P64">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>47.27359467028986</v>
       </c>
     </row>
@@ -41098,19 +41098,19 @@
         <v>11</v>
       </c>
       <c r="M65">
-        <f>F62/0.46</f>
+        <f t="shared" si="16"/>
         <v>243.5886956521739</v>
       </c>
       <c r="N65">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2435.8869565217392</v>
       </c>
       <c r="O65">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2466.1406725217389</v>
       </c>
       <c r="P65">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>41.10234454202898</v>
       </c>
     </row>
@@ -41149,19 +41149,19 @@
         <v>11</v>
       </c>
       <c r="M66">
-        <f>F63/0.46</f>
+        <f t="shared" si="16"/>
         <v>239.18413043478259</v>
       </c>
       <c r="N66">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2391.8413043478258</v>
       </c>
       <c r="O66">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2421.547973347826</v>
       </c>
       <c r="P66">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>40.359132889130436</v>
       </c>
     </row>
@@ -41200,19 +41200,19 @@
         <v>11</v>
       </c>
       <c r="M67">
-        <f>F64/0.46</f>
+        <f t="shared" si="16"/>
         <v>361.47434782608696</v>
       </c>
       <c r="N67">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>3614.7434782608698</v>
       </c>
       <c r="O67">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>3659.6385922608692</v>
       </c>
       <c r="P67">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>60.993976537681156</v>
       </c>
     </row>
@@ -41251,19 +41251,19 @@
         <v>11</v>
       </c>
       <c r="M68">
-        <f>F65/0.46</f>
+        <f t="shared" si="16"/>
         <v>278.53456521739128</v>
       </c>
       <c r="N68">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2785.3456521739126</v>
       </c>
       <c r="O68">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2819.9396451739126</v>
       </c>
       <c r="P68">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>46.998994086231875</v>
       </c>
     </row>
@@ -41302,19 +41302,19 @@
         <v>11</v>
       </c>
       <c r="M69">
-        <f>F66/0.46</f>
+        <f t="shared" si="16"/>
         <v>233.08260869565217</v>
       </c>
       <c r="N69">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2330.8260869565215</v>
       </c>
       <c r="O69">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2359.7749469565219</v>
       </c>
       <c r="P69">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>39.329582449275364</v>
       </c>
     </row>
@@ -41353,19 +41353,19 @@
         <v>11</v>
       </c>
       <c r="M70">
-        <f>F67/0.46</f>
+        <f t="shared" si="16"/>
         <v>325.04173913043479</v>
       </c>
       <c r="N70">
-        <f t="shared" ref="N70:N76" si="14">M70*10</f>
+        <f t="shared" ref="N70:N76" si="18">M70*10</f>
         <v>3250.4173913043478</v>
       </c>
       <c r="O70">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>3290.7875753043477</v>
       </c>
       <c r="P70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>54.846459588405793</v>
       </c>
     </row>
@@ -41404,19 +41404,19 @@
         <v>11</v>
       </c>
       <c r="M71">
-        <f>F68/0.46</f>
+        <f t="shared" si="16"/>
         <v>318.05347826086955</v>
       </c>
       <c r="N71">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3180.5347826086954</v>
       </c>
       <c r="O71">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>3220.0370246086954</v>
       </c>
       <c r="P71">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>53.667283743478258</v>
       </c>
     </row>
@@ -41455,19 +41455,19 @@
         <v>11</v>
       </c>
       <c r="M72">
-        <f>F69/0.46</f>
+        <f t="shared" si="16"/>
         <v>252.04673913043479</v>
       </c>
       <c r="N72">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2520.467391304348</v>
       </c>
       <c r="O72">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2551.7715963043479</v>
       </c>
       <c r="P72">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>42.529526605072462</v>
       </c>
     </row>
@@ -41506,19 +41506,19 @@
         <v>11</v>
       </c>
       <c r="M73">
-        <f>F70/0.46</f>
+        <f t="shared" si="16"/>
         <v>284.14260869565214</v>
       </c>
       <c r="N73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2841.4260869565214</v>
       </c>
       <c r="O73">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2876.7165989565215</v>
       </c>
       <c r="P73">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>47.945276649275357</v>
       </c>
     </row>
@@ -41557,19 +41557,19 @@
         <v>11</v>
       </c>
       <c r="M74">
-        <f>F71/0.46</f>
+        <f t="shared" si="16"/>
         <v>200.20304347826087</v>
       </c>
       <c r="N74">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2002.0304347826086</v>
       </c>
       <c r="O74">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2026.8956527826087</v>
       </c>
       <c r="P74">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>33.781594213043476</v>
       </c>
     </row>
@@ -41608,19 +41608,19 @@
         <v>11</v>
       </c>
       <c r="M75">
-        <f>F72/0.46</f>
+        <f t="shared" si="16"/>
         <v>347.875</v>
       </c>
       <c r="N75">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>3478.75</v>
       </c>
       <c r="O75">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>3521.9560750000001</v>
       </c>
       <c r="P75">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>58.69926791666667</v>
       </c>
     </row>
@@ -41659,19 +41659,19 @@
         <v>11</v>
       </c>
       <c r="M76">
-        <f>F73/0.46</f>
+        <f t="shared" si="16"/>
         <v>271.21695652173912</v>
       </c>
       <c r="N76">
-        <f t="shared" si="14"/>
+        <f t="shared" si="18"/>
         <v>2712.1695652173912</v>
       </c>
       <c r="O76">
-        <f t="shared" si="13"/>
+        <f t="shared" si="17"/>
         <v>2745.854711217391</v>
       </c>
       <c r="P76">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>45.764245186956515</v>
       </c>
     </row>

</xml_diff>